<commit_message>
Update submodule references after auto-commits
</commit_message>
<xml_diff>
--- a/build/test.xlsx
+++ b/build/test.xlsx
@@ -1,46 +1,121 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView activeTab="1" xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Meetings" sheetId="1" r:id="rId1"/>
+    <sheet name="2025" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Hello, world!</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Today:</t>
+  </si>
+  <si>
+    <t>Sobriety Date:</t>
+  </si>
+  <si>
+    <t>Sober Days:</t>
+  </si>
+  <si>
+    <t>Sober Weeks:</t>
+  </si>
+  <si>
+    <t>Sober Months:</t>
+  </si>
+  <si>
+    <t>Sober Years:</t>
+  </si>
+  <si>
+    <t>7:30a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="0">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -48,18 +123,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF505050"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="12" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -325,17 +427,166 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5078125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.97265625" bestFit="1" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.97265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1">
+        <f>TODAY()</f>
+        <v>45881</v>
+      </c>
+      <c r="C1" s="3">
+        <v>365.2242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45778</v>
+      </c>
+      <c r="C2" s="4">
+        <f>C1/ 12</f>
+        <v>30.43535</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="8">
+        <f>B1-B2</f>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2">
+        <f>B3/ 7</f>
+        <v>14.7142857142857</v>
+      </c>
+      <c r="C4" s="5">
+        <f>B3/ 7</f>
+        <v>14.7142857142857</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2">
+        <f>B3/ (365.2242 / 12)</f>
+        <v>3.38422262270682</v>
+      </c>
+      <c r="C5" s="5">
+        <f>B3/C2</f>
+        <v>3.38422262270682</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <f>B3/C1</f>
+        <v>0.282018551892235</v>
+      </c>
+      <c r="C6" s="5">
+        <f>B3/C1</f>
+        <v>0.282018551892235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.03515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.03515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.95703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.8984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.03515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.03515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.03515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.3046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>